<commit_message>
fixed navbar and added 2 extra styles
</commit_message>
<xml_diff>
--- a/Logo_dimensions.xlsx
+++ b/Logo_dimensions.xlsx
@@ -8,18 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leahshepherd/MyThings/sydney-advanced-endo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C038390-1593-584E-A826-E963D2F97F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E13971-9ABB-9144-96E8-AB354892A700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{A65F4F35-88E9-5041-9F6F-93DC7DCDE3C1}"/>
+    <workbookView minimized="1" xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{A65F4F35-88E9-5041-9F6F-93DC7DCDE3C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$20:$C$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$21:$C$21</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -675,11 +671,11 @@
     </row>
     <row r="28" spans="1:11">
       <c r="J28">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K28">
         <f>J28*K24</f>
-        <v>72</v>
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>